<commit_message>
Save module into database from excel
</commit_message>
<xml_diff>
--- a/src/main/resources/file/SubjectPlan.xlsx
+++ b/src/main/resources/file/SubjectPlan.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/11C0523C43241A7D/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wong zhao xuan\Documents\Programming Languages\Java\Course Timetable\timetable\src\main\resources\file\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9E124CEA-EA93-4178-BB81-50A2E8D7B2B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A449DA1D-89D4-4D00-B8E1-AB3D5F3CE2CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28905" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{5F22BF39-1CB6-43E9-8B89-396B364E780A}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{5F22BF39-1CB6-43E9-8B89-396B364E780A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="175">
   <si>
     <t>Subject Code</t>
   </si>
@@ -140,9 +140,6 @@
     <t>MTH1114</t>
   </si>
   <si>
-    <t>MTH2113 /MTH2103</t>
-  </si>
-  <si>
     <t>MU4 2422</t>
   </si>
   <si>
@@ -170,9 +167,6 @@
     <t>NET1014</t>
   </si>
   <si>
-    <t>CSC120</t>
-  </si>
-  <si>
     <t>PRG2104</t>
   </si>
   <si>
@@ -414,6 +408,159 @@
   </si>
   <si>
     <t>Project Management</t>
+  </si>
+  <si>
+    <t>Software Architecture and Design Patterns</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Data Mining and Knowledge Discovery </t>
+  </si>
+  <si>
+    <t>Business Intelligence System</t>
+  </si>
+  <si>
+    <t>Programming Principles</t>
+  </si>
+  <si>
+    <t>Computer Organisation</t>
+  </si>
+  <si>
+    <t>CSC1202</t>
+  </si>
+  <si>
+    <t>Digital Image Processing</t>
+  </si>
+  <si>
+    <t>Data Strcuture and Algorithmns</t>
+  </si>
+  <si>
+    <t>Operation System Fundamentals</t>
+  </si>
+  <si>
+    <t>Human Computer Interaction</t>
+  </si>
+  <si>
+    <t>Computational Intelligence</t>
+  </si>
+  <si>
+    <t>Computer Security</t>
+  </si>
+  <si>
+    <t>Database Engineering</t>
+  </si>
+  <si>
+    <t>Artificial Intelligence</t>
+  </si>
+  <si>
+    <t>Enterprise Architecture</t>
+  </si>
+  <si>
+    <t>Startup Foundry</t>
+  </si>
+  <si>
+    <t>Introduction to Statistics</t>
+  </si>
+  <si>
+    <t>Analytics Engineering</t>
+  </si>
+  <si>
+    <t>Web and Networks Analytics</t>
+  </si>
+  <si>
+    <t>IS Management and Strategy</t>
+  </si>
+  <si>
+    <t>Micro-credential in Computer Mathematics Fundamentals</t>
+  </si>
+  <si>
+    <t>Multimedia Networking</t>
+  </si>
+  <si>
+    <t>Computer Mathematics</t>
+  </si>
+  <si>
+    <t>Probability and Statistics</t>
+  </si>
+  <si>
+    <t>Community Service</t>
+  </si>
+  <si>
+    <t>Networking Principle</t>
+  </si>
+  <si>
+    <t>Data Communication</t>
+  </si>
+  <si>
+    <t>Computer Networks</t>
+  </si>
+  <si>
+    <t>Network Security</t>
+  </si>
+  <si>
+    <t>Distributed Systems</t>
+  </si>
+  <si>
+    <t>Network Management</t>
+  </si>
+  <si>
+    <t>Object-Oriented Programming</t>
+  </si>
+  <si>
+    <t>Object-Oriented Programming Fundamentals</t>
+  </si>
+  <si>
+    <t>Programming Languages</t>
+  </si>
+  <si>
+    <t>Functional Programming Principles</t>
+  </si>
+  <si>
+    <t>Enterprise Application Development</t>
+  </si>
+  <si>
+    <t>Capstone Project 1</t>
+  </si>
+  <si>
+    <t>Capstone Project 2</t>
+  </si>
+  <si>
+    <t>Advanced Network Security</t>
+  </si>
+  <si>
+    <t>Computer Hacking Forensic Investigator</t>
+  </si>
+  <si>
+    <t>Database Fundamentals</t>
+  </si>
+  <si>
+    <t>Database Management Systems</t>
+  </si>
+  <si>
+    <t>Software Engineering</t>
+  </si>
+  <si>
+    <t>Internship</t>
+  </si>
+  <si>
+    <t>Requirement Engineering</t>
+  </si>
+  <si>
+    <t>Code Camp</t>
+  </si>
+  <si>
+    <t>Software Testing</t>
+  </si>
+  <si>
+    <t>Software Evolution and Maintenance</t>
+  </si>
+  <si>
+    <t>Web Fundamentals</t>
+  </si>
+  <si>
+    <t>Web Programming</t>
+  </si>
+  <si>
+    <t>MTH2113/MTH2103</t>
   </si>
 </sst>
 </file>
@@ -790,8 +937,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DF822B5-23A8-403D-B407-6B49E5230FB2}">
   <dimension ref="A1:K56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -845,7 +992,7 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>10</v>
@@ -874,7 +1021,7 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>13</v>
@@ -906,7 +1053,7 @@
         <v>12</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C4" s="1" t="b">
         <v>1</v>
@@ -924,10 +1071,10 @@
         <v>7</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
@@ -935,7 +1082,7 @@
         <v>16</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C5" s="1" t="b">
         <v>1</v>
@@ -953,10 +1100,10 @@
         <v>42</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
@@ -964,7 +1111,7 @@
         <v>17</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C6" s="1" t="b">
         <v>1</v>
@@ -985,13 +1132,16 @@
         <v>11</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>18</v>
       </c>
+      <c r="B7" s="1" t="s">
+        <v>125</v>
+      </c>
       <c r="C7" s="1" t="b">
         <v>1</v>
       </c>
@@ -1008,15 +1158,18 @@
         <v>134</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>126</v>
       </c>
       <c r="C8" s="1" t="b">
         <v>1</v>
@@ -1034,15 +1187,18 @@
         <v>122</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>127</v>
       </c>
       <c r="C9" s="1" t="b">
         <v>1</v>
@@ -1060,15 +1216,18 @@
         <v>287</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>44</v>
+        <v>129</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>128</v>
       </c>
       <c r="C10" s="1" t="b">
         <v>1</v>
@@ -1086,16 +1245,19 @@
         <v>407</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>19</v>
       </c>
+      <c r="B11" s="1" t="s">
+        <v>130</v>
+      </c>
       <c r="C11" s="1" t="b">
         <v>1</v>
       </c>
@@ -1112,16 +1274,19 @@
         <v>78</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>20</v>
       </c>
+      <c r="B12" s="1" t="s">
+        <v>131</v>
+      </c>
       <c r="C12" s="1" t="b">
         <v>1</v>
       </c>
@@ -1138,15 +1303,18 @@
         <v>81</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>132</v>
       </c>
       <c r="C13" s="1" t="b">
         <v>1</v>
@@ -1164,16 +1332,19 @@
         <v>269</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>21</v>
       </c>
+      <c r="B14" s="1" t="s">
+        <v>133</v>
+      </c>
       <c r="C14" s="1" t="b">
         <v>1</v>
       </c>
@@ -1190,16 +1361,19 @@
         <v>134</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>22</v>
       </c>
+      <c r="B15" s="1" t="s">
+        <v>134</v>
+      </c>
       <c r="C15" s="1" t="b">
         <v>1</v>
       </c>
@@ -1216,16 +1390,19 @@
         <v>89</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>23</v>
       </c>
+      <c r="B16" s="1" t="s">
+        <v>135</v>
+      </c>
       <c r="C16" s="1" t="b">
         <v>1</v>
       </c>
@@ -1242,16 +1419,19 @@
         <v>40</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>24</v>
       </c>
+      <c r="B17" s="1" t="s">
+        <v>136</v>
+      </c>
       <c r="C17" s="1" t="b">
         <v>1</v>
       </c>
@@ -1268,16 +1448,19 @@
         <v>68</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>26</v>
       </c>
+      <c r="B18" s="1" t="s">
+        <v>137</v>
+      </c>
       <c r="C18" s="1" t="b">
         <v>1</v>
       </c>
@@ -1294,16 +1477,19 @@
         <v>34</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>25</v>
       </c>
+      <c r="B19" s="1" t="s">
+        <v>124</v>
+      </c>
       <c r="C19" s="1" t="b">
         <v>1</v>
       </c>
@@ -1320,16 +1506,19 @@
         <v>17</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>27</v>
       </c>
+      <c r="B20" s="1" t="s">
+        <v>138</v>
+      </c>
       <c r="C20" s="1" t="b">
         <v>1</v>
       </c>
@@ -1346,15 +1535,18 @@
         <v>49</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>139</v>
       </c>
       <c r="C21" s="1" t="b">
         <v>1</v>
@@ -1372,15 +1564,18 @@
         <v>230</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>140</v>
       </c>
       <c r="C22" s="1" t="b">
         <v>1</v>
@@ -1398,19 +1593,22 @@
         <v>13</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>28</v>
       </c>
+      <c r="B23" s="1" t="s">
+        <v>141</v>
+      </c>
       <c r="C23" s="1" t="b">
         <v>1</v>
       </c>
@@ -1427,16 +1625,19 @@
         <v>128</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>29</v>
       </c>
+      <c r="B24" s="1" t="s">
+        <v>142</v>
+      </c>
       <c r="C24" s="1" t="b">
         <v>1</v>
       </c>
@@ -1453,16 +1654,19 @@
         <v>83</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>30</v>
       </c>
+      <c r="B25" s="1" t="s">
+        <v>143</v>
+      </c>
       <c r="C25" s="1" t="b">
         <v>1</v>
       </c>
@@ -1479,16 +1683,19 @@
         <v>48</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>31</v>
       </c>
+      <c r="B26" s="1" t="s">
+        <v>144</v>
+      </c>
       <c r="C26" s="1" t="b">
         <v>1</v>
       </c>
@@ -1505,16 +1712,19 @@
         <v>38</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="J26" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>32</v>
       </c>
+      <c r="B27" s="1" t="s">
+        <v>145</v>
+      </c>
       <c r="C27" s="1" t="b">
         <v>1</v>
       </c>
@@ -1531,16 +1741,19 @@
         <v>36</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>33</v>
       </c>
+      <c r="B28" s="1" t="s">
+        <v>146</v>
+      </c>
       <c r="C28" s="1" t="b">
         <v>1</v>
       </c>
@@ -1557,15 +1770,18 @@
         <v>312</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="J28" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
-        <v>34</v>
+        <v>174</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>147</v>
       </c>
       <c r="C29" s="1" t="b">
         <v>1</v>
@@ -1583,15 +1799,18 @@
         <v>10</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="J29" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>148</v>
       </c>
       <c r="C30" s="1" t="b">
         <v>1</v>
@@ -1609,12 +1828,15 @@
         <v>115</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>149</v>
       </c>
       <c r="C31" s="1" t="b">
         <v>1</v>
@@ -1632,15 +1854,18 @@
         <v>268</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="I31" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>150</v>
       </c>
       <c r="C32" s="1" t="b">
         <v>1</v>
@@ -1658,15 +1883,18 @@
         <v>134</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="J32" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>151</v>
       </c>
       <c r="C33" s="1" t="b">
         <v>1</v>
@@ -1684,15 +1912,18 @@
         <v>193</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>152</v>
       </c>
       <c r="C34" s="1" t="b">
         <v>1</v>
@@ -1710,15 +1941,18 @@
         <v>63</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>153</v>
       </c>
       <c r="C35" s="1" t="b">
         <v>1</v>
@@ -1736,15 +1970,18 @@
         <v>310</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="I35" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>154</v>
       </c>
       <c r="C36" s="1" t="b">
         <v>1</v>
@@ -1762,15 +1999,18 @@
         <v>145</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="I36" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>156</v>
       </c>
       <c r="C37" s="1" t="b">
         <v>1</v>
@@ -1788,15 +2028,18 @@
         <v>161</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="I37" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>155</v>
       </c>
       <c r="C38" s="1" t="b">
         <v>1</v>
@@ -1814,15 +2057,18 @@
         <v>43</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="I38" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>157</v>
       </c>
       <c r="C39" s="1" t="b">
         <v>1</v>
@@ -1840,15 +2086,18 @@
         <v>121</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="I39" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>158</v>
       </c>
       <c r="C40" s="1" t="b">
         <v>1</v>
@@ -1866,15 +2115,18 @@
         <v>83</v>
       </c>
       <c r="H40" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="I40" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>159</v>
       </c>
       <c r="C41" s="1" t="b">
         <v>1</v>
@@ -1892,15 +2144,18 @@
         <v>16</v>
       </c>
       <c r="H41" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="I41" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>160</v>
       </c>
       <c r="C42" s="1" t="b">
         <v>1</v>
@@ -1918,12 +2173,15 @@
         <v>276</v>
       </c>
       <c r="H42" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>161</v>
       </c>
       <c r="C43" s="1" t="b">
         <v>0</v>
@@ -1941,12 +2199,15 @@
         <v>316</v>
       </c>
       <c r="H43" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>162</v>
       </c>
       <c r="C44" s="1" t="b">
         <v>1</v>
@@ -1964,15 +2225,18 @@
         <v>49</v>
       </c>
       <c r="H44" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="I44" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>163</v>
       </c>
       <c r="C45" s="1" t="b">
         <v>1</v>
@@ -1990,15 +2254,18 @@
         <v>117</v>
       </c>
       <c r="H45" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="I45" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>162</v>
       </c>
       <c r="C46" s="1" t="b">
         <v>1</v>
@@ -2016,15 +2283,18 @@
         <v>50</v>
       </c>
       <c r="H46" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="I46" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>164</v>
       </c>
       <c r="C47" s="1" t="b">
         <v>1</v>
@@ -2042,15 +2312,18 @@
         <v>318</v>
       </c>
       <c r="H47" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="I47" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>165</v>
       </c>
       <c r="C48" s="1" t="b">
         <v>1</v>
@@ -2068,15 +2341,18 @@
         <v>94</v>
       </c>
       <c r="H48" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="I48" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>166</v>
       </c>
       <c r="C49" s="1" t="b">
         <v>1</v>
@@ -2094,15 +2370,18 @@
         <v>6</v>
       </c>
       <c r="H49" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="I49" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>167</v>
       </c>
       <c r="C50" s="1" t="b">
         <v>0</v>
@@ -2120,12 +2399,15 @@
         <v>14</v>
       </c>
       <c r="H50" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>168</v>
       </c>
       <c r="C51" s="1" t="b">
         <v>1</v>
@@ -2143,15 +2425,18 @@
         <v>83</v>
       </c>
       <c r="H51" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="I51" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>169</v>
       </c>
       <c r="C52" s="1" t="b">
         <v>1</v>
@@ -2169,15 +2454,18 @@
         <v>54</v>
       </c>
       <c r="H52" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>170</v>
       </c>
       <c r="C53" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D53" s="1" t="b">
         <v>0</v>
@@ -2192,15 +2480,18 @@
         <v>112</v>
       </c>
       <c r="H53" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="J53" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>171</v>
       </c>
       <c r="C54" s="1" t="b">
         <v>1</v>
@@ -2218,15 +2509,18 @@
         <v>59</v>
       </c>
       <c r="H54" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="J54" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>172</v>
       </c>
       <c r="C55" s="1" t="b">
         <v>1</v>
@@ -2244,15 +2538,18 @@
         <v>239</v>
       </c>
       <c r="H55" s="1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="I55" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>173</v>
       </c>
       <c r="C56" s="1" t="b">
         <v>1</v>
@@ -2270,10 +2567,10 @@
         <v>86</v>
       </c>
       <c r="H56" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="I56" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Save programme into database from excel
</commit_message>
<xml_diff>
--- a/src/main/resources/file/SubjectPlan.xlsx
+++ b/src/main/resources/file/SubjectPlan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wong zhao xuan\Documents\Programming Languages\Java\Course Timetable\timetable\src\main\resources\file\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A449DA1D-89D4-4D00-B8E1-AB3D5F3CE2CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{675F5098-3F29-4C78-AFD1-00E3EF35DFA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{5F22BF39-1CB6-43E9-8B89-396B364E780A}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="177">
   <si>
     <t>Subject Code</t>
   </si>
@@ -47,9 +47,6 @@
     <t>Lecturer</t>
   </si>
   <si>
-    <t>PraticalTutor</t>
-  </si>
-  <si>
     <t>TutorialTutor</t>
   </si>
   <si>
@@ -59,9 +56,6 @@
     <t>Total Estimated Students</t>
   </si>
   <si>
-    <t>Pratical</t>
-  </si>
-  <si>
     <t>Tutorial</t>
   </si>
   <si>
@@ -122,9 +116,6 @@
     <t>EAC2014</t>
   </si>
   <si>
-    <t>IST12034</t>
-  </si>
-  <si>
     <t>IST2334</t>
   </si>
   <si>
@@ -561,6 +552,21 @@
   </si>
   <si>
     <t>MTH2113/MTH2103</t>
+  </si>
+  <si>
+    <t>IST2034</t>
+  </si>
+  <si>
+    <t>Advanced Topics in Computer Security</t>
+  </si>
+  <si>
+    <t>Lecture</t>
+  </si>
+  <si>
+    <t>PracticalTutor</t>
+  </si>
+  <si>
+    <t>Practical</t>
   </si>
 </sst>
 </file>
@@ -935,10 +941,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DF822B5-23A8-403D-B407-6B49E5230FB2}">
-  <dimension ref="A1:K56"/>
+  <dimension ref="A1:K58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -963,39 +969,39 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>174</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="G1" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>4</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C2" s="1" t="b">
         <v>1</v>
@@ -1013,18 +1019,18 @@
         <v>120</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C3" s="1" t="b">
         <v>1</v>
@@ -1042,18 +1048,18 @@
         <v>49</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="C4" s="1" t="b">
         <v>1</v>
@@ -1071,18 +1077,18 @@
         <v>7</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="C5" s="1" t="b">
         <v>1</v>
@@ -1100,18 +1106,18 @@
         <v>42</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C6" s="1" t="b">
         <v>1</v>
@@ -1129,18 +1135,18 @@
         <v>101</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C7" s="1" t="b">
         <v>1</v>
@@ -1158,18 +1164,18 @@
         <v>134</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="C8" s="1" t="b">
         <v>1</v>
@@ -1187,18 +1193,18 @@
         <v>122</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="C9" s="1" t="b">
         <v>1</v>
@@ -1216,18 +1222,18 @@
         <v>287</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="C10" s="1" t="b">
         <v>1</v>
@@ -1245,18 +1251,18 @@
         <v>407</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="C11" s="1" t="b">
         <v>1</v>
@@ -1274,18 +1280,18 @@
         <v>78</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="C12" s="1" t="b">
         <v>1</v>
@@ -1303,18 +1309,18 @@
         <v>81</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C13" s="1" t="b">
         <v>1</v>
@@ -1332,18 +1338,18 @@
         <v>269</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="C14" s="1" t="b">
         <v>1</v>
@@ -1361,18 +1367,18 @@
         <v>134</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="C15" s="1" t="b">
         <v>1</v>
@@ -1390,18 +1396,18 @@
         <v>89</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C16" s="1" t="b">
         <v>1</v>
@@ -1419,18 +1425,18 @@
         <v>40</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="C17" s="1" t="b">
         <v>1</v>
@@ -1448,18 +1454,18 @@
         <v>68</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="C18" s="1" t="b">
         <v>1</v>
@@ -1477,18 +1483,18 @@
         <v>34</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C19" s="1" t="b">
         <v>1</v>
@@ -1506,18 +1512,18 @@
         <v>17</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="C20" s="1" t="b">
         <v>1</v>
@@ -1535,18 +1541,18 @@
         <v>49</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="C21" s="1" t="b">
         <v>1</v>
@@ -1564,18 +1570,18 @@
         <v>230</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="C22" s="1" t="b">
         <v>1</v>
@@ -1593,21 +1599,21 @@
         <v>13</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>28</v>
+        <v>172</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="C23" s="1" t="b">
         <v>1</v>
@@ -1625,18 +1631,18 @@
         <v>128</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="C24" s="1" t="b">
         <v>1</v>
@@ -1654,18 +1660,18 @@
         <v>83</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="C25" s="1" t="b">
         <v>1</v>
@@ -1683,18 +1689,18 @@
         <v>48</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="C26" s="1" t="b">
         <v>1</v>
@@ -1712,18 +1718,18 @@
         <v>38</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="J26" s="1" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="C27" s="1" t="b">
         <v>1</v>
@@ -1741,18 +1747,18 @@
         <v>36</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="C28" s="1" t="b">
         <v>1</v>
@@ -1770,18 +1776,18 @@
         <v>312</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="J28" s="1" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="C29" s="1" t="b">
         <v>1</v>
@@ -1799,18 +1805,18 @@
         <v>10</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="J29" s="1" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="C30" s="1" t="b">
         <v>1</v>
@@ -1828,15 +1834,15 @@
         <v>115</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="C31" s="1" t="b">
         <v>1</v>
@@ -1854,18 +1860,18 @@
         <v>268</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="I31" s="1" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="C32" s="1" t="b">
         <v>1</v>
@@ -1883,18 +1889,18 @@
         <v>134</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="J32" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C33" s="1" t="b">
         <v>1</v>
@@ -1912,18 +1918,18 @@
         <v>193</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="C34" s="1" t="b">
         <v>1</v>
@@ -1941,18 +1947,18 @@
         <v>63</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="C35" s="1" t="b">
         <v>1</v>
@@ -1970,18 +1976,18 @@
         <v>310</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="I35" s="1" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="C36" s="1" t="b">
         <v>1</v>
@@ -1999,18 +2005,18 @@
         <v>145</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="I36" s="1" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="C37" s="1" t="b">
         <v>1</v>
@@ -2028,18 +2034,18 @@
         <v>161</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="I37" s="1" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C38" s="1" t="b">
         <v>1</v>
@@ -2057,18 +2063,18 @@
         <v>43</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="I38" s="1" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="C39" s="1" t="b">
         <v>1</v>
@@ -2086,18 +2092,18 @@
         <v>121</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="I39" s="1" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="C40" s="1" t="b">
         <v>1</v>
@@ -2115,18 +2121,18 @@
         <v>83</v>
       </c>
       <c r="H40" s="1" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="I40" s="1" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="C41" s="1" t="b">
         <v>1</v>
@@ -2144,18 +2150,18 @@
         <v>16</v>
       </c>
       <c r="H41" s="1" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="I41" s="1" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="C42" s="1" t="b">
         <v>1</v>
@@ -2173,15 +2179,15 @@
         <v>276</v>
       </c>
       <c r="H42" s="1" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="C43" s="1" t="b">
         <v>0</v>
@@ -2199,15 +2205,15 @@
         <v>316</v>
       </c>
       <c r="H43" s="1" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="C44" s="1" t="b">
         <v>1</v>
@@ -2225,18 +2231,18 @@
         <v>49</v>
       </c>
       <c r="H44" s="1" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="I44" s="1" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="C45" s="1" t="b">
         <v>1</v>
@@ -2254,18 +2260,18 @@
         <v>117</v>
       </c>
       <c r="H45" s="1" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="I45" s="1" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>162</v>
+        <v>173</v>
       </c>
       <c r="C46" s="1" t="b">
         <v>1</v>
@@ -2283,18 +2289,18 @@
         <v>50</v>
       </c>
       <c r="H46" s="1" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="I46" s="1" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="C47" s="1" t="b">
         <v>1</v>
@@ -2312,18 +2318,18 @@
         <v>318</v>
       </c>
       <c r="H47" s="1" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="I47" s="1" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="C48" s="1" t="b">
         <v>1</v>
@@ -2341,18 +2347,18 @@
         <v>94</v>
       </c>
       <c r="H48" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="I48" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="C49" s="1" t="b">
         <v>1</v>
@@ -2370,18 +2376,18 @@
         <v>6</v>
       </c>
       <c r="H49" s="1" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="I49" s="1" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="C50" s="1" t="b">
         <v>0</v>
@@ -2399,15 +2405,15 @@
         <v>14</v>
       </c>
       <c r="H50" s="1" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="C51" s="1" t="b">
         <v>1</v>
@@ -2425,18 +2431,18 @@
         <v>83</v>
       </c>
       <c r="H51" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="I51" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="C52" s="1" t="b">
         <v>1</v>
@@ -2454,15 +2460,15 @@
         <v>54</v>
       </c>
       <c r="H52" s="1" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="C53" s="1" t="b">
         <v>1</v>
@@ -2480,18 +2486,18 @@
         <v>112</v>
       </c>
       <c r="H53" s="1" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="J53" s="1" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="C54" s="1" t="b">
         <v>1</v>
@@ -2509,18 +2515,18 @@
         <v>59</v>
       </c>
       <c r="H54" s="1" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="J54" s="1" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C55" s="1" t="b">
         <v>1</v>
@@ -2538,18 +2544,18 @@
         <v>239</v>
       </c>
       <c r="H55" s="1" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="I55" s="1" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="C56" s="1" t="b">
         <v>1</v>
@@ -2567,10 +2573,16 @@
         <v>86</v>
       </c>
       <c r="H56" s="1" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="I56" s="1" t="s">
-        <v>120</v>
+        <v>117</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G58" s="1">
+        <f>SUM(G2:G56)</f>
+        <v>6551</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Apply Constraint Programming technique for scheduling timeslot
</commit_message>
<xml_diff>
--- a/src/main/resources/file/SubjectPlan.xlsx
+++ b/src/main/resources/file/SubjectPlan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wong zhao xuan\Documents\Programming Languages\Java\Course Timetable\timetable\src\main\resources\file\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{675F5098-3F29-4C78-AFD1-00E3EF35DFA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B096DE8-179C-4BD4-AF24-2E69D5B95C2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{5F22BF39-1CB6-43E9-8B89-396B364E780A}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="178">
   <si>
     <t>Subject Code</t>
   </si>
@@ -567,6 +567,9 @@
   </si>
   <si>
     <t>Practical</t>
+  </si>
+  <si>
+    <t>Dr Sathishkumar VE</t>
   </si>
 </sst>
 </file>
@@ -943,8 +946,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DF822B5-23A8-403D-B407-6B49E5230FB2}">
   <dimension ref="A1:K58"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1106,10 +1109,10 @@
         <v>42</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>66</v>
+        <v>177</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>66</v>
+        <v>177</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">

</xml_diff>